<commit_message>
all test done and the design passed !!
</commit_message>
<xml_diff>
--- a/DV paln.xlsx
+++ b/DV paln.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/640c7b691a6cc924/Desktop/DV/CX-301-A2 _ FIFO Layared Testbench/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaser\OneDrive\Desktop\DV\CX-301-A2 _ FIFO Layared Testbench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{7ABC9738-ADE2-4829-8302-B45A7944FB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE690C2C-3938-4BE8-B78E-CD58BDD1D3D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EB394A-9F83-4A55-873F-0BC72A4D9488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{C7323C7C-AF83-40F4-B6C3-076CA88F89E3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{C7323C7C-AF83-40F4-B6C3-076CA88F89E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -59,18 +59,12 @@
     <t>write when fifo is full</t>
   </si>
   <si>
-    <t>read when fifo is empty</t>
-  </si>
-  <si>
     <t>Ranadom</t>
   </si>
   <si>
     <t xml:space="preserve">Directed </t>
   </si>
   <si>
-    <t>Reset FIFO</t>
-  </si>
-  <si>
     <t>empty FIFO</t>
   </si>
   <si>
@@ -95,37 +89,34 @@
     <t xml:space="preserve">Not Executed </t>
   </si>
   <si>
-    <t>Push five random data values into the FIFO (32-bit width, depth = 10) and read them back to ensure correct behavior.</t>
-  </si>
-  <si>
-    <t>Reset FIFO:
-1.Fill the FIFO and check the empty flag.
-2.Reset after reaseting the FIFO.
-3, Reset the FIFO when a transaction passes between classes (passed if the transaction is skipped).</t>
-  </si>
-  <si>
     <t>Push random data into the FIFO until full, then verify the full flag.</t>
   </si>
   <si>
     <t>Fill the FIFO, then attempt to read from it (pass if the full flag is cleared).</t>
   </si>
   <si>
-    <t>Fill the FIFO, then attempt to write to it to verify design behavior.</t>
-  </si>
-  <si>
-    <t>Read from the FIFO until it is empty, then check the empty flag.</t>
-  </si>
-  <si>
     <t>Empty the FIFO, then attempt to write to it (pass if the full flag is cleared).</t>
   </si>
   <si>
-    <t>Read from the FIFO until it is empty, then attempt another read to verify design behavior.</t>
-  </si>
-  <si>
     <t>Push 10 random data values into the FIFO (64-bit width, depth = 10) and read them back to ensure correct behavior.</t>
   </si>
   <si>
     <t>X_item</t>
+  </si>
+  <si>
+    <t>Push five random data values into the FIFO (8-bit width, depth = 8) and read them back to ensure correct behavior.</t>
+  </si>
+  <si>
+    <t>Fill the FIFO, then attempt to write to it one more time,  after that read all the content of fifo (pass if the last write is dropped) .</t>
+  </si>
+  <si>
+    <t>wirte randomeRead from the FIFO until it is empty, then check the empty flag.</t>
+  </si>
+  <si>
+    <t>done on v_item</t>
+  </si>
+  <si>
+    <t>I change the parameters then applay the v_item test and it passed !!</t>
   </si>
 </sst>
 </file>
@@ -258,10 +249,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481CC62A-2005-41A1-A779-C6C6DF417B00}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -595,7 +582,7 @@
     <col min="4" max="4" width="41.53125" customWidth="1"/>
     <col min="5" max="5" width="15.86328125" customWidth="1"/>
     <col min="6" max="6" width="18.265625" customWidth="1"/>
-    <col min="7" max="7" width="34.9296875" customWidth="1"/>
+    <col min="7" max="7" width="42.33203125" customWidth="1"/>
     <col min="12" max="12" width="19.46484375" customWidth="1"/>
     <col min="21" max="21" width="26.6640625" customWidth="1"/>
   </cols>
@@ -626,16 +613,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -648,20 +635,20 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2"/>
       <c r="T3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -670,23 +657,23 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="G4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -695,20 +682,20 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2"/>
       <c r="U5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="35" customHeight="1" x14ac:dyDescent="0.45">
@@ -717,18 +704,20 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="35" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
@@ -736,73 +725,49 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" ht="35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
@@ -814,35 +779,22 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="B12" s="1"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{60D75ACF-ABEA-4B4A-9E99-8143C3BDD34E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E13 E2:E8" xr:uid="{60D75ACF-ABEA-4B4A-9E99-8143C3BDD34E}">
       <formula1>$T$3:$T$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{D3475688-0ED4-4947-B1E4-DD9E0983A918}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8" xr:uid="{D3475688-0ED4-4947-B1E4-DD9E0983A918}">
       <formula1>$U$3:$U$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -889,7 +841,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F2:F10</xm:sqref>
+          <xm:sqref>F2:F8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="7" operator="containsText" id="{64C58376-1876-4A8E-ADC7-2504BEA0F0AE}">

</xml_diff>